<commit_message>
update hkd yc bootstrapping
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC1MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="18765" yWindow="-15" windowWidth="18825" windowHeight="11460"/>
+    <workbookView xWindow="18765" yWindow="-15" windowWidth="18825" windowHeight="11460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
   <si>
     <t>Earliest Date</t>
   </si>
@@ -502,6 +502,27 @@
   </si>
   <si>
     <t>1M</t>
+  </si>
+  <si>
+    <t>HKD_YC1MRH_AM1H2M</t>
+  </si>
+  <si>
+    <t>HKD_YC1MRH_AM1H4M</t>
+  </si>
+  <si>
+    <t>HKD_YC1MRH_AM1H5M</t>
+  </si>
+  <si>
+    <t>HKD_YC1MRH_AM1H7M</t>
+  </si>
+  <si>
+    <t>HKD_YC1MRH_AM1H8M</t>
+  </si>
+  <si>
+    <t>HKD_YC1MRH_AM1H10M</t>
+  </si>
+  <si>
+    <t>HKD_YC1MRH_AM1H11M</t>
   </si>
 </sst>
 </file>
@@ -1430,6 +1451,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1452,10 +1477,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="3"/>
@@ -1768,7 +1789,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1790,19 +1811,19 @@
       </c>
     </row>
     <row r="2" spans="1:30" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="131"/>
-      <c r="H2" s="132" t="s">
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
+      <c r="H2" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="134"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1842,7 +1863,7 @@
       <c r="C4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="137">
+      <c r="D4" s="129">
         <v>1</v>
       </c>
       <c r="E4" s="4"/>
@@ -1853,7 +1874,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="74">
-        <v>41598.708865740744</v>
+        <v>41598.736087962963</v>
       </c>
       <c r="K4" s="82"/>
       <c r="L4" s="1"/>
@@ -2000,7 +2021,7 @@
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="138" t="s">
+      <c r="C8" s="130" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="11" t="str">
@@ -2083,7 +2104,7 @@
       </c>
       <c r="D10" s="14" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC1M#0006</v>
+        <v>_HKDYC1M#0002</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
@@ -2162,12 +2183,12 @@
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="132" t="s">
+      <c r="H12" s="134" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="134"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="136"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -4096,6 +4117,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4234,7 +4256,7 @@
       </c>
       <c r="L4" s="111" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_xAM1H_Hibor1M#0006</v>
+        <v>HKD_YC1MRH_xAM1H_Hibor1M#0001</v>
       </c>
       <c r="M4" s="110" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -4310,7 +4332,7 @@
       </c>
       <c r="L6" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H2M#0006</v>
+        <v>HKD_YC1MRH_AM1H2M#0001</v>
       </c>
       <c r="M6" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -4355,7 +4377,7 @@
       </c>
       <c r="L7" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H3M#0006</v>
+        <v>HKD_YC1MRH_AM1H3M#0001</v>
       </c>
       <c r="M7" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -4400,7 +4422,7 @@
       </c>
       <c r="L8" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H4M#0006</v>
+        <v>HKD_YC1MRH_AM1H4M#0001</v>
       </c>
       <c r="M8" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -4445,7 +4467,7 @@
       </c>
       <c r="L9" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H5M#0006</v>
+        <v>HKD_YC1MRH_AM1H5M#0001</v>
       </c>
       <c r="M9" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -4490,7 +4512,7 @@
       </c>
       <c r="L10" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H6M#0006</v>
+        <v>HKD_YC1MRH_AM1H6M#0001</v>
       </c>
       <c r="M10" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -4535,7 +4557,7 @@
       </c>
       <c r="L11" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H7M#0006</v>
+        <v>HKD_YC1MRH_AM1H7M#0001</v>
       </c>
       <c r="M11" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -4580,7 +4602,7 @@
       </c>
       <c r="L12" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H8M#0006</v>
+        <v>HKD_YC1MRH_AM1H8M#0001</v>
       </c>
       <c r="M12" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -4625,7 +4647,7 @@
       </c>
       <c r="L13" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H9M#0006</v>
+        <v>HKD_YC1MRH_AM1H9M#0001</v>
       </c>
       <c r="M13" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -4670,7 +4692,7 @@
       </c>
       <c r="L14" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H10M#0006</v>
+        <v>HKD_YC1MRH_AM1H10M#0001</v>
       </c>
       <c r="M14" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -4715,7 +4737,7 @@
       </c>
       <c r="L15" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H11M#0006</v>
+        <v>HKD_YC1MRH_AM1H11M#0001</v>
       </c>
       <c r="M15" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -4760,7 +4782,7 @@
       </c>
       <c r="L16" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H1Y#0006</v>
+        <v>HKD_YC1MRH_AM1H1Y#0001</v>
       </c>
       <c r="M16" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -4829,7 +4851,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4869,9 +4891,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K6</f>
-        <v>HKD_YC1MRH_AM1H2M</v>
+      <c r="A2" s="124" t="s">
+        <v>100</v>
       </c>
       <c r="B2" s="62" t="e">
         <f>_xll.qlRateHelperQuoteValue($A2,Trigger)</f>
@@ -4907,9 +4928,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K7</f>
-        <v>HKD_YC1MRH_AM1H3M</v>
+      <c r="A3" s="124" t="s">
+        <v>62</v>
       </c>
       <c r="B3" s="62">
         <f>_xll.qlRateHelperQuoteValue($A3,Trigger)</f>
@@ -4945,9 +4965,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K8</f>
-        <v>HKD_YC1MRH_AM1H4M</v>
+      <c r="A4" s="124" t="s">
+        <v>101</v>
       </c>
       <c r="B4" s="62" t="e">
         <f>_xll.qlRateHelperQuoteValue($A4,Trigger)</f>
@@ -4983,9 +5002,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K9</f>
-        <v>HKD_YC1MRH_AM1H5M</v>
+      <c r="A5" s="124" t="s">
+        <v>102</v>
       </c>
       <c r="B5" s="62" t="e">
         <f>_xll.qlRateHelperQuoteValue($A5,Trigger)</f>
@@ -5021,9 +5039,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K10</f>
-        <v>HKD_YC1MRH_AM1H6M</v>
+      <c r="A6" s="124" t="s">
+        <v>63</v>
       </c>
       <c r="B6" s="62">
         <f>_xll.qlRateHelperQuoteValue($A6,Trigger)</f>
@@ -5059,9 +5076,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K11</f>
-        <v>HKD_YC1MRH_AM1H7M</v>
+      <c r="A7" s="124" t="s">
+        <v>103</v>
       </c>
       <c r="B7" s="62" t="e">
         <f>_xll.qlRateHelperQuoteValue($A7,Trigger)</f>
@@ -5097,9 +5113,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K12</f>
-        <v>HKD_YC1MRH_AM1H8M</v>
+      <c r="A8" s="124" t="s">
+        <v>104</v>
       </c>
       <c r="B8" s="62" t="e">
         <f>_xll.qlRateHelperQuoteValue($A8,Trigger)</f>
@@ -5135,9 +5150,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K13</f>
-        <v>HKD_YC1MRH_AM1H9M</v>
+      <c r="A9" s="124" t="s">
+        <v>64</v>
       </c>
       <c r="B9" s="62">
         <f>_xll.qlRateHelperQuoteValue($A9,Trigger)</f>
@@ -5167,9 +5181,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K14</f>
-        <v>HKD_YC1MRH_AM1H10M</v>
+      <c r="A10" s="124" t="s">
+        <v>105</v>
       </c>
       <c r="B10" s="62" t="e">
         <f>_xll.qlRateHelperQuoteValue($A10,Trigger)</f>
@@ -5199,9 +5212,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="124" t="str">
-        <f>HKD_YCRH_Swaps_1M!K15</f>
-        <v>HKD_YC1MRH_AM1H11M</v>
+      <c r="A11" s="124" t="s">
+        <v>106</v>
       </c>
       <c r="B11" s="62" t="e">
         <f>_xll.qlRateHelperQuoteValue($A11,Trigger)</f>
@@ -5231,9 +5243,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="125" t="str">
-        <f>HKD_YCRH_Swaps_1M!K16</f>
-        <v>HKD_YC1MRH_AM1H1Y</v>
+      <c r="A12" s="125" t="s">
+        <v>65</v>
       </c>
       <c r="B12" s="66">
         <f>_xll.qlRateHelperQuoteValue($A12,Trigger)</f>
@@ -5296,10 +5307,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="136"/>
+      <c r="B1" s="138"/>
       <c r="D1" s="35" t="s">
         <v>20</v>
       </c>
@@ -5512,7 +5523,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D13),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_RateHelpersSelected#0006</v>
+        <v>HKD_YC1MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>

</xml_diff>

<commit_message>
create trigger to make ratehelperselection dependent on ratehelper constructors
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC1MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="18765" yWindow="-15" windowWidth="18825" windowHeight="11460" activeTab="2"/>
+    <workbookView xWindow="18765" yWindow="-15" windowWidth="18825" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <definedName name="ObjectOverwrite">'General Settings'!$J$6</definedName>
     <definedName name="Permanent">'General Settings'!$J$5</definedName>
     <definedName name="QuoteSuffix">'General Settings'!$J$19</definedName>
+    <definedName name="RateHelperConstructors" localSheetId="1">HKD_YCRH_Swaps_1M!$L$6:$L$16</definedName>
     <definedName name="RateHelperPrefix">'General Settings'!$D$8</definedName>
     <definedName name="RateHelpers">RateHelpers!$A$2:$A$12</definedName>
     <definedName name="RateHelpersIncluded">RateHelpers!$D$2:$D$12</definedName>
@@ -1789,7 +1790,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1874,7 +1875,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="74">
-        <v>41598.736087962963</v>
+        <v>41599.409618055557</v>
       </c>
       <c r="K4" s="82"/>
       <c r="L4" s="1"/>
@@ -2104,7 +2105,7 @@
       </c>
       <c r="D10" s="14" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC1M#0002</v>
+        <v>_HKDYC1M#0001</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
@@ -2612,7 +2613,7 @@
       <c r="B23" s="2"/>
       <c r="C23" s="56">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41598</v>
+        <v>41599</v>
       </c>
       <c r="D23" s="28">
         <f>MAX(_xll.ohPack(Selected!I1:I13))</f>
@@ -2650,11 +2651,11 @@
       <c r="B24" s="2"/>
       <c r="C24" s="57">
         <f>MAX(_xll.ohPack(Selected!H2:H13))</f>
-        <v>41967</v>
+        <v>41968</v>
       </c>
       <c r="D24" s="10">
         <f>MIN(_xll.ohPack(Selected!I1:I13))</f>
-        <v>0.99718199621706238</v>
+        <v>0.99718723822049571</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
@@ -4120,7 +4121,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4256,7 +4259,7 @@
       </c>
       <c r="L4" s="111" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_xAM1H_Hibor1M#0001</v>
+        <v>HKD_YC1MRH_xAM1H_Hibor1M#0000</v>
       </c>
       <c r="M4" s="110" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -4332,7 +4335,7 @@
       </c>
       <c r="L6" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H2M#0001</v>
+        <v>HKD_YC1MRH_AM1H2M#0000</v>
       </c>
       <c r="M6" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -4377,7 +4380,7 @@
       </c>
       <c r="L7" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H3M#0001</v>
+        <v>HKD_YC1MRH_AM1H3M#0000</v>
       </c>
       <c r="M7" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -4422,7 +4425,7 @@
       </c>
       <c r="L8" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H4M#0001</v>
+        <v>HKD_YC1MRH_AM1H4M#0000</v>
       </c>
       <c r="M8" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -4467,7 +4470,7 @@
       </c>
       <c r="L9" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H5M#0001</v>
+        <v>HKD_YC1MRH_AM1H5M#0000</v>
       </c>
       <c r="M9" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -4512,7 +4515,7 @@
       </c>
       <c r="L10" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H6M#0001</v>
+        <v>HKD_YC1MRH_AM1H6M#0000</v>
       </c>
       <c r="M10" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -4557,7 +4560,7 @@
       </c>
       <c r="L11" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H7M#0001</v>
+        <v>HKD_YC1MRH_AM1H7M#0000</v>
       </c>
       <c r="M11" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -4602,7 +4605,7 @@
       </c>
       <c r="L12" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H8M#0001</v>
+        <v>HKD_YC1MRH_AM1H8M#0000</v>
       </c>
       <c r="M12" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -4647,7 +4650,7 @@
       </c>
       <c r="L13" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H9M#0001</v>
+        <v>HKD_YC1MRH_AM1H9M#0000</v>
       </c>
       <c r="M13" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -4692,7 +4695,7 @@
       </c>
       <c r="L14" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H10M#0001</v>
+        <v>HKD_YC1MRH_AM1H10M#0000</v>
       </c>
       <c r="M14" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -4737,7 +4740,7 @@
       </c>
       <c r="L15" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H11M#0001</v>
+        <v>HKD_YC1MRH_AM1H11M#0000</v>
       </c>
       <c r="M15" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -4782,7 +4785,7 @@
       </c>
       <c r="L16" s="101" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_AM1H1Y#0001</v>
+        <v>HKD_YC1MRH_AM1H1Y#0000</v>
       </c>
       <c r="M16" s="100" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -4851,7 +4854,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4914,11 +4917,11 @@
       </c>
       <c r="G2" s="64">
         <f>_xll.qlRateHelperEarliestDate($A2,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H2" s="65">
         <f>_xll.qlRateHelperLatestDate($A2,Trigger)</f>
-        <v>41661</v>
+        <v>41666</v>
       </c>
       <c r="I2" s="34">
         <v>10</v>
@@ -4951,11 +4954,11 @@
       </c>
       <c r="G3" s="64">
         <f>_xll.qlRateHelperEarliestDate($A3,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H3" s="65">
         <f>_xll.qlRateHelperLatestDate($A3,Trigger)</f>
-        <v>41694</v>
+        <v>41695</v>
       </c>
       <c r="I3" s="34">
         <v>20</v>
@@ -4988,11 +4991,11 @@
       </c>
       <c r="G4" s="64">
         <f>_xll.qlRateHelperEarliestDate($A4,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H4" s="65">
         <f>_xll.qlRateHelperLatestDate($A4,Trigger)</f>
-        <v>41722</v>
+        <v>41723</v>
       </c>
       <c r="I4" s="34">
         <v>30</v>
@@ -5025,11 +5028,11 @@
       </c>
       <c r="G5" s="64">
         <f>_xll.qlRateHelperEarliestDate($A5,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H5" s="65">
         <f>_xll.qlRateHelperLatestDate($A5,Trigger)</f>
-        <v>41751</v>
+        <v>41754</v>
       </c>
       <c r="I5" s="34">
         <v>40</v>
@@ -5062,11 +5065,11 @@
       </c>
       <c r="G6" s="64">
         <f>_xll.qlRateHelperEarliestDate($A6,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H6" s="65">
         <f>_xll.qlRateHelperLatestDate($A6,Trigger)</f>
-        <v>41781</v>
+        <v>41785</v>
       </c>
       <c r="I6" s="34">
         <v>50</v>
@@ -5099,11 +5102,11 @@
       </c>
       <c r="G7" s="64">
         <f>_xll.qlRateHelperEarliestDate($A7,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H7" s="65">
         <f>_xll.qlRateHelperLatestDate($A7,Trigger)</f>
-        <v>41813</v>
+        <v>41815</v>
       </c>
       <c r="I7" s="34">
         <v>60</v>
@@ -5136,11 +5139,11 @@
       </c>
       <c r="G8" s="64">
         <f>_xll.qlRateHelperEarliestDate($A8,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H8" s="65">
         <f>_xll.qlRateHelperLatestDate($A8,Trigger)</f>
-        <v>41842</v>
+        <v>41845</v>
       </c>
       <c r="I8" s="34">
         <v>70</v>
@@ -5173,11 +5176,11 @@
       </c>
       <c r="G9" s="64">
         <f>_xll.qlRateHelperEarliestDate($A9,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H9" s="65">
         <f>_xll.qlRateHelperLatestDate($A9,Trigger)</f>
-        <v>41873</v>
+        <v>41876</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -5204,11 +5207,11 @@
       </c>
       <c r="G10" s="64">
         <f>_xll.qlRateHelperEarliestDate($A10,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H10" s="65">
         <f>_xll.qlRateHelperLatestDate($A10,Trigger)</f>
-        <v>41904</v>
+        <v>41907</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -5235,11 +5238,11 @@
       </c>
       <c r="G11" s="64">
         <f>_xll.qlRateHelperEarliestDate($A11,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H11" s="65">
         <f>_xll.qlRateHelperLatestDate($A11,Trigger)</f>
-        <v>41934</v>
+        <v>41939</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -5266,11 +5269,11 @@
       </c>
       <c r="G12" s="68">
         <f>_xll.qlRateHelperEarliestDate($A12,Trigger)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H12" s="69">
         <f>_xll.qlRateHelperLatestDate($A12,Trigger)</f>
-        <v>41967</v>
+        <v>41968</v>
       </c>
     </row>
   </sheetData>
@@ -5343,7 +5346,7 @@
         <v>62</v>
       </c>
       <c r="D2" s="41" t="str">
-        <f t="array" ref="D2:D13">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
+        <f t="array" ref="D2:D13">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),ISERROR(HKD_YCRH_Swaps_1M!RateHelperConstructors))</f>
         <v>HKD_YC1MRH_AM1H3M</v>
       </c>
       <c r="E2" s="42">
@@ -5356,14 +5359,14 @@
       </c>
       <c r="G2" s="43">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H2" s="44">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41694</v>
+        <v>41695</v>
       </c>
       <c r="I2" s="38">
-        <v>0.99944888117593667</v>
+        <v>0.99944973191562592</v>
       </c>
       <c r="K2" s="34">
         <v>2.1000000000000003E-3</v>
@@ -5395,14 +5398,14 @@
       </c>
       <c r="G3" s="43">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H3" s="44">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41781</v>
+        <v>41785</v>
       </c>
       <c r="I3" s="38">
-        <v>0.99880069538760774</v>
+        <v>0.99878357775957516</v>
       </c>
       <c r="K3" s="34">
         <v>2.3999999999999998E-3</v>
@@ -5434,14 +5437,14 @@
       </c>
       <c r="G4" s="43">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H4" s="44">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41873</v>
+        <v>41876</v>
       </c>
       <c r="I4" s="38">
-        <v>0.99804854241953556</v>
+        <v>0.99803828918481163</v>
       </c>
       <c r="K4" s="34">
         <v>2.5999999999999999E-3</v>
@@ -5473,14 +5476,14 @@
       </c>
       <c r="G5" s="43">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41600</v>
+        <v>41603</v>
       </c>
       <c r="H5" s="44">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41967</v>
+        <v>41968</v>
       </c>
       <c r="I5" s="38">
-        <v>0.99718199621706238</v>
+        <v>0.99718723822049571</v>
       </c>
       <c r="K5" s="34">
         <v>2.8000000000000004E-3</v>
@@ -5523,7 +5526,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D13),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC1MRH_RateHelpersSelected#0002</v>
+        <v>HKD_YC1MRH_RateHelpersSelected#0001</v>
       </c>
       <c r="B7" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>

</xml_diff>